<commit_message>
Charac order def added
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -340,12 +340,447 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>44849.1702769601</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>44849.17028125414</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>44849.17028504426</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>44849.17028956416</v>
+      </c>
+      <c r="I1">
+        <v>2</v>
+      </c>
+      <c r="J1">
+        <v>44849.17029423401</v>
+      </c>
+      <c r="K1">
+        <v>-22</v>
+      </c>
+      <c r="L1">
+        <v>44849.17029766271</v>
+      </c>
+      <c r="M1">
+        <v>18</v>
+      </c>
+      <c r="N1">
+        <v>44849.17030127547</v>
+      </c>
+      <c r="O1">
+        <v>50</v>
+      </c>
+      <c r="P1">
+        <v>44849.170305616</v>
+      </c>
+      <c r="Q1">
+        <v>-2</v>
+      </c>
+      <c r="R1">
+        <v>44849.1703089094</v>
+      </c>
+      <c r="S1">
+        <v>352</v>
+      </c>
+      <c r="T1">
+        <v>44849.17031216991</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2">
+        <v>-398</v>
+      </c>
+      <c r="B2">
+        <v>44849.17031733906</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>44849.17032120964</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>44849.17032490917</v>
+      </c>
+      <c r="G2">
+        <v>-4</v>
+      </c>
+      <c r="H2">
+        <v>44849.17032849523</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>44849.17033180952</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>44849.1703351231</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>44849.17033861856</v>
+      </c>
+      <c r="O2">
+        <v>-14</v>
+      </c>
+      <c r="P2">
+        <v>44849.17034209623</v>
+      </c>
+      <c r="Q2">
+        <v>4</v>
+      </c>
+      <c r="R2">
+        <v>44849.1703455008</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>44849.17034881293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>44849.17035267346</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>44849.17035602457</v>
+      </c>
+      <c r="E3">
+        <v>-4</v>
+      </c>
+      <c r="F3">
+        <v>44849.1703593356</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>44849.17036289652</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>44849.17036660483</v>
+      </c>
+      <c r="K3">
+        <v>166</v>
+      </c>
+      <c r="L3">
+        <v>44849.17036996749</v>
+      </c>
+      <c r="M3">
+        <v>-12</v>
+      </c>
+      <c r="N3">
+        <v>44849.17037349453</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>44849.17037695866</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>44849.17038031066</v>
+      </c>
+      <c r="S3">
+        <v>14</v>
+      </c>
+      <c r="T3">
+        <v>44849.17038386717</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>44849.17038769923</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>44849.17039103554</v>
+      </c>
+      <c r="E4">
+        <v>-154</v>
+      </c>
+      <c r="F4">
+        <v>44849.17039444794</v>
+      </c>
+      <c r="G4">
+        <v>-4</v>
+      </c>
+      <c r="H4">
+        <v>44849.17039821513</v>
+      </c>
+      <c r="I4">
+        <v>-2</v>
+      </c>
+      <c r="J4">
+        <v>44849.17040160018</v>
+      </c>
+      <c r="K4">
+        <v>160</v>
+      </c>
+      <c r="L4">
+        <v>44849.17040493352</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>44849.17040841785</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>44849.17041186405</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>44849.17041528501</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>44849.17041867029</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>44849.17042230105</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>44849.17042564927</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>44849.17042893967</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>44849.17043263917</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>44849.17043595208</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>44849.17043932354</v>
+      </c>
+      <c r="M5">
+        <v>-160</v>
+      </c>
+      <c r="N5">
+        <v>44849.17044292567</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>44849.17044645846</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>44849.17044978323</v>
+      </c>
+      <c r="S5">
+        <v>-8</v>
+      </c>
+      <c r="T5">
+        <v>44849.17045311193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>44849.17045678266</v>
+      </c>
+      <c r="C6">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>44849.17046004816</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>44849.17046335697</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>44849.17046678947</v>
+      </c>
+      <c r="I6">
+        <v>-6</v>
+      </c>
+      <c r="J6">
+        <v>44849.17047019549</v>
+      </c>
+      <c r="K6">
+        <v>220</v>
+      </c>
+      <c r="L6">
+        <v>44849.17047364602</v>
+      </c>
+      <c r="M6">
+        <v>-218</v>
+      </c>
+      <c r="N6">
+        <v>44849.17047693115</v>
+      </c>
+      <c r="O6">
+        <v>-4</v>
+      </c>
+      <c r="P6">
+        <v>44849.17048051656</v>
+      </c>
+      <c r="Q6">
+        <v>-2</v>
+      </c>
+      <c r="R6">
+        <v>44849.17048383989</v>
+      </c>
+      <c r="S6">
+        <v>-6</v>
+      </c>
+      <c r="T6">
+        <v>44849.17048710585</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>44849.17049094972</v>
+      </c>
+      <c r="C7">
+        <v>-6</v>
+      </c>
+      <c r="D7">
+        <v>44849.17049426262</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>44849.17049768065</v>
+      </c>
+      <c r="G7">
+        <v>-24</v>
+      </c>
+      <c r="H7">
+        <v>44849.17050120912</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>44849.17050463902</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>44849.17050795702</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>44849.17051137699</v>
+      </c>
+      <c r="O7">
+        <v>-14</v>
+      </c>
+      <c r="P7">
+        <v>44849.17051497785</v>
+      </c>
+      <c r="Q7">
+        <v>-2</v>
+      </c>
+      <c r="R7">
+        <v>44849.17051824775</v>
+      </c>
+      <c r="S7">
+        <v>6</v>
+      </c>
+      <c r="T7">
+        <v>44849.170521565</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>